<commit_message>
TODO: Step-sze Changed output of sceneNames so it's more compact.
</commit_message>
<xml_diff>
--- a/results/0926/2022-0926_resnet34_malmotest.xlsx
+++ b/results/0926/2022-0926_resnet34_malmotest.xlsx
@@ -540,37 +540,37 @@
       </c>
       <c r="I2" t="inlineStr">
         <is>
-          <t>['FloorPlan_Train1_1', 'FloorPlan_Train2_1', 'FloorPlan_Train3_1', 'FloorPlan_Train4_1', 'FloorPlan_Train5_1']</t>
+          <t>['FloorPlan_Train1_1', 'FloorPlan_Train2_1', 'FloorPlan_Train3_1', 'FloorPlan_Train4_1', 'FloorPlan_Train5_1', 'FloorPlan_Train6_1', 'FloorPlan_Train7_1', 'FloorPlan_Train8_1', 'FloorPlan_Train9_1', 'FloorPlan_Train10_1', 'FloorPlan_Train1_1', 'FloorPlan_Train2_1', 'FloorPlan_Train3_1', 'FloorPlan_Train4_1', 'FloorPlan_Train5_1', 'FloorPlan_Train6_1', 'FloorPlan_Train7_1', 'FloorPlan_Train8_1', 'FloorPlan_Train9_1', 'FloorPlan_Train10_1']</t>
         </is>
       </c>
       <c r="J2" t="inlineStr">
         <is>
-          <t>[81, 93, 103, 114, 148, 194]</t>
+          <t>[81, 93, 103, 114, 148, 194, 197, 197, 197, 197, 218, 220, 222, 240, 242, 293, 319, 319, 319, 319, 342]</t>
         </is>
       </c>
       <c r="K2" t="inlineStr">
         <is>
-          <t>[0.086, 0.086, 0.098, 0.096, 0.094, 0.092]</t>
+          <t>[0.086, 0.086, 0.098, 0.096, 0.094, 0.092, 0.092, 0.092, 0.092, 0.092, 0.092, 0.092, 0.092, 0.09, 0.09, 0.09, 0.1, 0.1, 0.1, 0.1, 0.1]</t>
         </is>
       </c>
       <c r="L2" t="inlineStr">
         <is>
-          <t>[0, 30, 60, 90, 120, 150]</t>
+          <t>[0, 30, 60, 90, 120, 150, 180, 210, 240, 270, 300, 330, 360, 390, 420, 450, 480, 510, 540, 570, 600]</t>
         </is>
       </c>
       <c r="M2" t="inlineStr">
         <is>
-          <t>[0, 16.097865295410166, 38.60830733776093, 61.87577478885649, 83.7264050245285, 106.24110400676727]</t>
+          <t>[0, 16.097865295410166, 38.60830733776093, 61.87577478885649, 83.7264050245285, 106.24110400676727, 113.78760421276093, 138.82562291622162, 151.63454074859618, 151.63454074859618, 160.57704050540923, 182.825630068779, 197.69045696258544, 219.51761140823365, 241.83314867019655, 267.2845475196839, 276.6690353274346, 303.59656013250355, 315.9621186614037, 315.9621186614037, 325.26231840848925]</t>
         </is>
       </c>
       <c r="N2" t="inlineStr">
         <is>
-          <t>[0, 0.36, 0.86, 1.36, 1.93, 2.48]</t>
+          <t>[0, 0.36, 0.86, 1.36, 1.93, 2.48, 3.06, 3.49, 3.98, 4.68, 5.11, 5.64, 6.21, 6.7, 7.61, 8.55, 9.45, 10.34, 11.35, 12.34, 13.03]</t>
         </is>
       </c>
       <c r="O2" t="inlineStr">
         <is>
-          <t>[0, -10, -10, 0, -10, -10, -10, -10, 0, -10, 0, 0, 0, -10, -10, -10, -10, -20, -20, 0, -20, 0, -20, 0, -20, -20, 0, 0, 0, -20, 0, 0, -20, -20, -20, 0, -20, 0, 0, -20, -10, -20, -20, -20, -20, -20, -20, -10, -20, 0, -10, 0, 0, 0, 0, 0, 0, 0, -10, 0, 0, -10, 0, 0, -10, 0, 0, 0, -10, 0, 0, -10, 0, -10, 0, 0, 0, 0, 0, 0, -20]</t>
+          <t>[0, -10, -10, 0, -10, -10, -10, -10, 0, -10, 0, 0, 0, -10, -10, -20, 0, -20, -20, 0, -20, 0, -20, 0, -20, -20, 0, 0, 0, -20, 0, 0, -20, -20, -20, 0, -20, 0, 0, -20, -10, -20, -20, -20, 0, -20, -20, -10, -20, 0, -10, 0, 0, 0, 0, 0, 0, 0, -10, 0, 0, 0, 0, 0, -10, -10, 0, -10, -10, 0, 0, -10, 0, -10, 0, 0, -10, 0, 0, 0, -20]</t>
         </is>
       </c>
     </row>
@@ -609,37 +609,37 @@
       </c>
       <c r="I3" t="inlineStr">
         <is>
-          <t>['FloorPlan_Train1_1', 'FloorPlan_Train2_1', 'FloorPlan_Train3_1', 'FloorPlan_Train4_1', 'FloorPlan_Train5_1']</t>
+          <t>['FloorPlan_Train1_1', 'FloorPlan_Train2_1', 'FloorPlan_Train3_1', 'FloorPlan_Train4_1', 'FloorPlan_Train5_1', 'FloorPlan_Train6_1', 'FloorPlan_Train7_1', 'FloorPlan_Train8_1', 'FloorPlan_Train9_1', 'FloorPlan_Train10_1', 'FloorPlan_Train1_1', 'FloorPlan_Train2_1', 'FloorPlan_Train3_1', 'FloorPlan_Train4_1', 'FloorPlan_Train5_1', 'FloorPlan_Train6_1', 'FloorPlan_Train7_1', 'FloorPlan_Train8_1', 'FloorPlan_Train9_1', 'FloorPlan_Train10_1']</t>
         </is>
       </c>
       <c r="J3" t="inlineStr">
         <is>
-          <t>[81, 85, 100, 113, 143, 192]</t>
+          <t>[81, 85, 100, 113, 143, 192, 213, 213, 213, 213, 237, 241, 244, 250, 275, 324, 347, 347, 347, 347, 393]</t>
         </is>
       </c>
       <c r="K3" t="inlineStr">
         <is>
-          <t>[0.342, 0.352, 0.374, 0.37, 0.382, 0.382]</t>
+          <t>[0.342, 0.352, 0.374, 0.37, 0.382, 0.382, 0.397, 0.397, 0.397, 0.397, 0.393, 0.398, 0.4, 0.4, 0.404, 0.404, 0.402, 0.402, 0.402, 0.402, 0.4]</t>
         </is>
       </c>
       <c r="L3" t="inlineStr">
         <is>
-          <t>[0, 30, 60, 90, 120, 150]</t>
+          <t>[0, 30, 60, 90, 120, 150, 180, 210, 240, 270, 300, 330, 360, 390, 420, 450, 480, 510, 540, 570, 600]</t>
         </is>
       </c>
       <c r="M3" t="inlineStr">
         <is>
-          <t>[0, 14.544830417633067, 38.229873919487005, 60.96841380596162, 81.42432296276094, 105.40737187862398]</t>
+          <t>[0, 14.544830417633067, 38.229873919487005, 60.96841380596162, 81.42432296276094, 105.40737187862398, 113.79237210750581, 134.84594135284428, 148.3509757995606, 148.3509757995606, 157.65117554664616, 178.0573615074158, 194.24799129962923, 219.1670227766037, 241.4825600385666, 266.9339588880539, 275.9897591352463, 302.9174396276474, 315.51484246253966, 315.51484246253966, 322.91660974025723]</t>
         </is>
       </c>
       <c r="N3" t="inlineStr">
         <is>
-          <t>[0, 0.03, 0.08, 0.11, 0.16, 0.23]</t>
+          <t>[0, 0.03, 0.08, 0.11, 0.16, 0.23, 0.28, 0.34, 0.39, 0.44, 0.5, 0.56, 0.63, 0.68, 0.75, 0.81, 0.9, 0.95, 1.01, 1.08, 1.14]</t>
         </is>
       </c>
       <c r="O3" t="inlineStr">
         <is>
-          <t>[0, -10, -10, 0, -10, -10, -10, -10, -10, -10, 0, 0, 0, -10, -10, -10, -20, -20, -20, 0, 0, 0, -20, 0, -20, -20, 0, -20, 0, -20, 0, 0, -20, -20, -20, 0, -20, 0, 0, -20, -10, -20, -20, -20, -20, -20, -10, -20, -10, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, 0, -10, -10, 0, 0, 0, 0, 0, -10, 0, -10, 0, -10, 0, 0, -10, 0, 0, 0, 0, 0, -20]</t>
+          <t>[0, -10, -10, 0, -10, -10, -10, -10, 0, -10, 0, 0, 0, -10, -10, -20, 0, -20, -20, 0, 0, 0, -20, 0, -20, -20, 0, 0, 0, -20, 0, 0, -20, -20, -20, 0, -20, 0, 0, -20, -10, -20, -20, -20, 0, -20, -20, -20, -10, 0, -20, -10, 0, 0, 0, 0, 0, 0, 0, -10, -10, -10, 0, 0, -10, -10, 0, 0, 0, 0, 0, -10, 0, 0, -10, 0, -10, 0, 0, 0, -20]</t>
         </is>
       </c>
     </row>
@@ -678,37 +678,37 @@
       </c>
       <c r="I4" t="inlineStr">
         <is>
-          <t>['FloorPlan_Train1_1', 'FloorPlan_Train2_1', 'FloorPlan_Train3_1', 'FloorPlan_Train4_1', 'FloorPlan_Train5_1']</t>
+          <t>['FloorPlan_Train1_1', 'FloorPlan_Train2_1', 'FloorPlan_Train3_1', 'FloorPlan_Train4_1', 'FloorPlan_Train5_1', 'FloorPlan_Train6_1', 'FloorPlan_Train7_1', 'FloorPlan_Train8_1', 'FloorPlan_Train9_1', 'FloorPlan_Train10_1', 'FloorPlan_Train11_1', 'FloorPlan_Train11_2', 'FloorPlan_Train11_3', 'FloorPlan_Train11_4', 'FloorPlan_Train11_5', 'FloorPlan_Train12_1', 'FloorPlan_Train12_2', 'FloorPlan_Train12_3', 'FloorPlan_Train12_4', 'FloorPlan_Train12_5']</t>
         </is>
       </c>
       <c r="J4" t="inlineStr">
         <is>
-          <t>[81, 84, 94, 102, 142, 189]</t>
+          <t>[81, 84, 94, 102, 142, 189, 190, 190, 190, 190, 210, 210, 210, 210, 210, 215, 218, 259, 306, 306, 329]</t>
         </is>
       </c>
       <c r="K4" t="inlineStr">
         <is>
-          <t>[0.086, 0.086, 0.092, 0.092, 0.094, 0.103]</t>
+          <t>[0.086, 0.086, 0.092, 0.092, 0.094, 0.103, 0.103, 0.103, 0.103, 0.103, 0.103, 0.103, 0.103, 0.103, 0.103, 0.103, 0.103, 0.109, 0.107, 0.107, 0.105]</t>
         </is>
       </c>
       <c r="L4" t="inlineStr">
         <is>
-          <t>[0, 30, 60, 90, 120, 150]</t>
+          <t>[0, 30, 60, 90, 120, 150, 180, 210, 240, 270, 300, 330, 360, 390, 420, 450, 480, 510, 540, 570, 600]</t>
         </is>
       </c>
       <c r="M4" t="inlineStr">
         <is>
-          <t>[0, 15.530802631378185, 37.09476878643035, 57.24029161930084, 77.69620077610017, 100.7003497362137]</t>
+          <t>[0, 15.530802631378185, 37.09476878643035, 57.24029161930084, 77.69620077610017, 100.7003497362137, 107.74374992847444, 132.30935318470003, 145.43205032348635, 145.43205032348635, 154.19570008516314, 175.495841896534, 192.57426539659502, 211.8608514428139, 235.58418039083483, 258.6813417553902, 275.4413020730019, 292.6162026047707, 307.3982270836831, 307.8179270863534, 328.02542659044275]</t>
         </is>
       </c>
       <c r="N4" t="inlineStr">
         <is>
-          <t>[0, 0.31, 0.67, 1.23, 2.04, 2.73]</t>
+          <t>[0, 0.31, 0.67, 1.23, 2.04, 2.73, 3.32, 3.81, 4.39, 4.78, 5.2, 5.58, 6.0, 6.52, 7.09, 7.61, 8.33, 9.29, 10.2, 11.25, 12.3]</t>
         </is>
       </c>
       <c r="O4" t="inlineStr">
         <is>
-          <t>[0, 0, 0, -10, -10, 0, 0, 0, 0, -10, -20, 0, 0, 0, -10, -10, 0, -10, 0, 0, -20, -10, -20, 0, 0, 0, -20, -20, -20, -10, 0, 0, -10, -20, -10, -10, -20, 0, -20, 0, -20, -20, -10, 0, -20, 0, 0, 0, -20, -20, 0, -10, -20, 0, 0, -20, 0, 0, 0, -20, 0, 0, 0, -10, 0, 0, 0, -10, 0, 0, -10, -20, -10, -10, 0, 0, 0, -20, -10, -20, -10]</t>
+          <t>[-10, 0, 0, -10, -20, 0, 0, -10, -20, 0, -10, 0, -20, -20, 0, 0, 0, 0, 0, -10, -10, 0, 0, 0, 0, 0, -20, -10, -10, 0, -10, -20, 0, 0, 0, -10, -20, -20, 0, 0, 0, 0, 0, 0, -20, 0, -20, -10, 0, -20, 0, 0, -10, 0, 0, 0, 0, -20, -20, 0, -20, -20, -10, 0, -20, 0, 0, -10, -10, -20, -10, -10, 0, 0, -20, -20, -10, -10, -20, -10, 0]</t>
         </is>
       </c>
     </row>
@@ -747,37 +747,37 @@
       </c>
       <c r="I5" t="inlineStr">
         <is>
-          <t>['FloorPlan_Train1_1', 'FloorPlan_Train2_1', 'FloorPlan_Train3_1', 'FloorPlan_Train4_1', 'FloorPlan_Train5_1']</t>
+          <t>['FloorPlan_Train1_1', 'FloorPlan_Train2_1', 'FloorPlan_Train3_1', 'FloorPlan_Train4_1', 'FloorPlan_Train5_1', 'FloorPlan_Train6_1', 'FloorPlan_Train7_1', 'FloorPlan_Train8_1', 'FloorPlan_Train9_1', 'FloorPlan_Train10_1', 'FloorPlan_Train1_4', 'FloorPlan_Train2_4', 'FloorPlan_Train3_4', 'FloorPlan_Train4_4', 'FloorPlan_Train5_4', 'FloorPlan_Train6_4', 'FloorPlan_Train7_4', 'FloorPlan_Train8_4', 'FloorPlan_Train9_4', 'FloorPlan_Train10_4']</t>
         </is>
       </c>
       <c r="J5" t="inlineStr">
         <is>
-          <t>[81, 87, 98, 104, 144, 192]</t>
+          <t>[81, 87, 98, 104, 144, 192, 214, 214, 214, 214, 223, 223, 227, 250, 252, 252, 252, 252, 252, 252, 252]</t>
         </is>
       </c>
       <c r="K5" t="inlineStr">
         <is>
-          <t>[0.342, 0.365, 0.389, 0.385, 0.383, 0.383]</t>
+          <t>[0.342, 0.365, 0.389, 0.385, 0.383, 0.383, 0.393, 0.393, 0.393, 0.393, 0.397, 0.397, 0.404, 0.41, 0.41, 0.41, 0.41, 0.41, 0.41, 0.41, 0.41]</t>
         </is>
       </c>
       <c r="L5" t="inlineStr">
         <is>
-          <t>[0, 30, 60, 90, 120, 150]</t>
+          <t>[0, 30, 60, 90, 120, 150, 180, 210, 240, 270, 300, 330, 360, 390, 420, 450, 480, 510, 540, 570, 600]</t>
         </is>
       </c>
       <c r="M5" t="inlineStr">
         <is>
-          <t>[0, 16.67876248359681, 38.05118577480316, 60.16182434558867, 80.61773350238799, 104.11133244037627]</t>
+          <t>[0, 16.67876248359681, 38.05118577480316, 60.16182434558867, 80.61773350238799, 104.11133244037627, 112.49633266925811, 138.0067668199539, 151.75726034641264, 151.75726034641264, 173.77884027361867, 201.77658314108845, 213.1931896626949, 237.1615375936031, 250.92134079337117, 273.1265073239803, 299.4534540593624, 320.50671071410176, 340.2187743127346, 361.99377297759054, 368.4016011893749]</t>
         </is>
       </c>
       <c r="N5" t="inlineStr">
         <is>
-          <t>[0, 0.04, 0.07, 0.1, 0.13, 0.18]</t>
+          <t>[0, 0.04, 0.07, 0.1, 0.13, 0.18, 0.23, 0.29, 0.35, 0.42, 0.46, 0.51, 0.6, 0.69, 0.75, 0.81, 0.86, 0.91, 0.97, 1.06, 1.13]</t>
         </is>
       </c>
       <c r="O5" t="inlineStr">
         <is>
-          <t>[0, 0, 0, -10, -10, 0, 0, 0, 0, -10, -20, 0, 0, 0, -10, -10, 0, -10, 0, 0, -20, -10, -20, 0, 0, 0, -20, -20, -20, -10, 0, 0, -10, -20, -10, -10, -20, 0, -20, 0, -20, -20, -10, 0, -20, 0, 0, 0, -20, -20, 0, -10, -20, 0, 0, -20, 0, 0, 0, -20, 0, 0, 0, -10, 0, 0, 0, -10, 0, 0, -10, -20, -10, -10, 0, 0, 0, -20, -10, -20, -10]</t>
+          <t>[-10, 0, -10, -20, -10, 0, -20, 0, 0, -10, -20, 0, 0, 0, -10, 0, 0, 0, 0, 0, -20, 0, -20, 0, -20, 0, 0, -20, -20, 0, 0, -20, 0, 0, 0, -10, -10, -20, 0, 0, 0, -10, -10, -20, 0, -20, 0, -20, 0, 0, -10, -10, 0, 0, -20, 0, -10, 0, 0, 0, 0, -10, -20, 0, -20, -10, -10, -10, -10, -20, 0, 0, 0, -10, -10, 0, -20, -20, -20, 0, -10]</t>
         </is>
       </c>
     </row>

</xml_diff>